<commit_message>
Edit rmarkdown thesis file, add reference list
</commit_message>
<xml_diff>
--- a/Data/Hyp & inclusion_Hyp/inclusion_Hyp.xlsx
+++ b/Data/Hyp & inclusion_Hyp/inclusion_Hyp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EliseSchramkowski\Documents\GitHub\thesis\Data\Hyp &amp; inclusion_Hyp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA04E99-BB36-4C4B-8BFA-30D6465581EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC894983-D545-4B45-81FC-66582D7F1B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15600" yWindow="3120" windowWidth="15120" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2673,8 +2673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L325"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
small changes + raw data
Final changes to thesis file, small, inconsequential changes to data set files, newer, cleaned up version of code. Also added raw data files for AllP and APA
</commit_message>
<xml_diff>
--- a/Data/Hyp & inclusion_Hyp/inclusion_Hyp.xlsx
+++ b/Data/Hyp & inclusion_Hyp/inclusion_Hyp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EliseSchramkowski\Documents\GitHub\thesis\Data\Hyp &amp; inclusion_Hyp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC894983-D545-4B45-81FC-66582D7F1B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F00ACB0-4E4B-4782-BE57-4E8F3A2C95A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15600" yWindow="3120" windowWidth="15120" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Articles" sheetId="1" r:id="rId1"/>
@@ -2058,7 +2058,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2119,14 +2119,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2148,7 +2140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2356,7 +2348,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2673,8 +2664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A315" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="F112" sqref="F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6141,32 +6132,32 @@
       <c r="J114" s="4"/>
       <c r="K114" s="4"/>
     </row>
-    <row r="115" spans="1:11" s="201" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="201" t="s">
+    <row r="115" spans="1:11" s="200" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="200" t="s">
         <v>333</v>
       </c>
-      <c r="B115" s="201" t="s">
+      <c r="B115" s="200" t="s">
         <v>308</v>
       </c>
-      <c r="C115" s="201" t="s">
-        <v>3</v>
-      </c>
-      <c r="D115" s="201">
+      <c r="C115" s="200" t="s">
+        <v>3</v>
+      </c>
+      <c r="D115" s="200">
         <v>2016</v>
       </c>
-      <c r="E115" s="201">
+      <c r="E115" s="200">
         <v>5</v>
       </c>
-      <c r="F115" s="201">
-        <v>0</v>
-      </c>
-      <c r="G115" s="201">
-        <v>0</v>
-      </c>
-      <c r="H115" s="201">
-        <v>0</v>
-      </c>
-      <c r="I115" s="201" t="s">
+      <c r="F115" s="200">
+        <v>0</v>
+      </c>
+      <c r="G115" s="200">
+        <v>0</v>
+      </c>
+      <c r="H115" s="200">
+        <v>0</v>
+      </c>
+      <c r="I115" s="200" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>